<commit_message>
Added meeting notes from 11/10/2018
</commit_message>
<xml_diff>
--- a/docs/gantt/gantt 10-16-18.xlsx
+++ b/docs/gantt/gantt 10-16-18.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748EEC30-B05B-4C67-ABC0-5B940B4B34D8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="415"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -22,29 +18,28 @@
     <definedName name="Scrolling_Increment">Gantt!$F$4</definedName>
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
   <si>
     <t>About This Template</t>
   </si>
@@ -363,11 +358,20 @@
   <si>
     <t>Unit Testing</t>
   </si>
+  <si>
+    <t>Sparh</t>
+  </si>
+  <si>
+    <t>Gage, Jacob, Zach</t>
+  </si>
+  <si>
+    <t>Thruster abstraction, Thruster Subclasses, animations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d"/>
@@ -901,6 +905,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,34 +955,12 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="9"/>
+    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
@@ -964,586 +968,20 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="46">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="165" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2124,18 +1562,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -2279,21 +1705,21 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="75"/>
-      <tableStyleElement type="headerRow" dxfId="74"/>
-      <tableStyleElement type="firstRowStripe" dxfId="73"/>
+    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="45"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="43"/>
     </tableStyle>
-    <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="72"/>
-      <tableStyleElement type="headerRow" dxfId="71"/>
-      <tableStyleElement type="totalRow" dxfId="70"/>
-      <tableStyleElement type="firstColumn" dxfId="69"/>
-      <tableStyleElement type="lastColumn" dxfId="68"/>
-      <tableStyleElement type="firstRowStripe" dxfId="67"/>
-      <tableStyleElement type="secondRowStripe" dxfId="66"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="65"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="64"/>
+    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="wholeTable" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="totalRow" dxfId="40"/>
+      <tableStyleElement type="firstColumn" dxfId="39"/>
+      <tableStyleElement type="lastColumn" dxfId="38"/>
+      <tableStyleElement type="firstRowStripe" dxfId="37"/>
+      <tableStyleElement type="secondRowStripe" dxfId="36"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="35"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="34"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2397,15 +1823,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>63</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2415,7 +1841,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2446,8 +1872,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
-  <autoFilter ref="B7:G68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
+  <autoFilter ref="B7:G68" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2456,12 +1882,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Milestone Description" dataDxfId="63"/>
-    <tableColumn id="2" name="Category" dataDxfId="62"/>
-    <tableColumn id="3" name="Assigned To" dataDxfId="61"/>
-    <tableColumn id="4" name="Progress"/>
-    <tableColumn id="5" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="6" name="No. Days" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone Description" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2473,13 +1899,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="60"/>
-    <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="Members"/>
-    <tableColumn id="4" name="Things Discussed"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Location"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Members"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Things Discussed"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2747,30 +2173,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BL71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A52" zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
       <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="64" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="64" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -2809,7 +2235,7 @@
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -2819,67 +2245,67 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="N2" s="61" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="N2" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="62" t="s">
+      <c r="S2" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="54" t="s">
+      <c r="AC2" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="53" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="58">
+      <c r="E3" s="64"/>
+      <c r="F3" s="66">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>43378</v>
       </c>
-      <c r="G3" s="59"/>
+      <c r="G3" s="67"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -2964,17 +2390,17 @@
       <c r="BK4" s="44"/>
       <c r="BL4" s="44"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>43378</v>
@@ -3200,7 +2626,7 @@
         <v>43433</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -3268,7 +2694,7 @@
       <c r="BK6" s="47"/>
       <c r="BL6" s="48"/>
     </row>
-    <row r="7" spans="1:64" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -3516,7 +2942,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -3583,7 +3009,7 @@
       <c r="BK8" s="36"/>
       <c r="BL8" s="36"/>
     </row>
-    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -3827,7 +3253,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="41" t="s">
         <v>29</v>
@@ -4073,7 +3499,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="52" t="s">
         <v>37</v>
@@ -4319,7 +3745,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="41" t="s">
         <v>30</v>
@@ -4565,7 +3991,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="41" t="s">
         <v>31</v>
@@ -4811,7 +4237,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="41" t="s">
         <v>32</v>
@@ -5057,7 +4483,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="41" t="s">
         <v>33</v>
@@ -5135,7 +4561,7 @@
       <c r="BK15" s="38"/>
       <c r="BL15" s="38"/>
     </row>
-    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="52" t="s">
         <v>34</v>
@@ -5381,7 +4807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="42" t="s">
         <v>28</v>
@@ -5623,7 +5049,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="41" t="s">
         <v>38</v>
@@ -5869,7 +5295,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="41" t="s">
         <v>39</v>
@@ -6115,7 +5541,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="41" t="s">
         <v>40</v>
@@ -6361,7 +5787,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="41" t="s">
         <v>41</v>
@@ -6607,7 +6033,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="52" t="s">
         <v>83</v>
@@ -6685,7 +6111,7 @@
       <c r="BK22" s="38"/>
       <c r="BL22" s="38"/>
     </row>
-    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="41" t="s">
         <v>42</v>
@@ -6931,7 +6357,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="52" t="s">
         <v>49</v>
@@ -7177,7 +6603,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="52" t="s">
         <v>50</v>
@@ -7255,7 +6681,7 @@
       <c r="BK25" s="38"/>
       <c r="BL25" s="38"/>
     </row>
-    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="41" t="s">
         <v>73</v>
@@ -7333,7 +6759,7 @@
       <c r="BK26" s="38"/>
       <c r="BL26" s="38"/>
     </row>
-    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="41" t="s">
         <v>74</v>
@@ -7411,7 +6837,7 @@
       <c r="BK27" s="38"/>
       <c r="BL27" s="38"/>
     </row>
-    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="52"/>
       <c r="C28" s="34"/>
@@ -7609,7 +7035,7 @@
         <v/>
       </c>
       <c r="BD28" s="38" t="str">
-        <f t="shared" ref="BD28:BL28" ca="1" si="13">IF(AND($C28="Goal",BD$5&gt;=$F28,BD$5&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",BD$5&gt;=$F28,BD$5&lt;=$F28+$G28-1),1,""))</f>
+        <f t="shared" ref="BD28" ca="1" si="13">IF(AND($C28="Goal",BD$5&gt;=$F28,BD$5&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",BD$5&gt;=$F28,BD$5&lt;=$F28+$G28-1),1,""))</f>
         <v/>
       </c>
       <c r="BE28" s="38" t="str">
@@ -7645,7 +7071,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="41"/>
       <c r="C29" s="34"/>
@@ -7879,7 +7305,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="42" t="s">
         <v>64</v>
@@ -8115,7 +7541,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="41" t="s">
         <v>58</v>
@@ -8361,7 +7787,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="41" t="s">
         <v>62</v>
@@ -8607,7 +8033,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="41" t="s">
         <v>65</v>
@@ -8853,7 +8279,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="41" t="s">
         <v>66</v>
@@ -9099,7 +8525,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="41" t="s">
         <v>67</v>
@@ -9345,7 +8771,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="41" t="s">
         <v>70</v>
@@ -9591,7 +9017,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="41" t="s">
         <v>68</v>
@@ -9837,9 +9263,9 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="65" t="s">
+      <c r="B38" s="55" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="34"/>
@@ -10075,9 +9501,9 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="55" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="34" t="s">
@@ -10321,9 +9747,9 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="55" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="34" t="s">
@@ -10567,7 +9993,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="41" t="s">
         <v>81</v>
@@ -10813,8 +10239,8 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:64" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="66"/>
+    <row r="42" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="56"/>
       <c r="B42" s="41" t="s">
         <v>82</v>
       </c>
@@ -10827,13 +10253,13 @@
       <c r="E42" s="30">
         <v>0</v>
       </c>
-      <c r="F42" s="70">
+      <c r="F42" s="60">
         <v>43395</v>
       </c>
-      <c r="G42" s="67">
+      <c r="G42" s="57">
         <v>28</v>
       </c>
-      <c r="H42" s="68"/>
+      <c r="H42" s="58"/>
       <c r="I42" s="38" t="str">
         <f t="shared" ca="1" si="11"/>
         <v/>
@@ -10923,7 +10349,7 @@
         <v/>
       </c>
       <c r="AE42" s="38" t="str">
-        <f t="shared" ref="AE42:AT42" ca="1" si="20">IF(AND($C42="Goal",AE$5&gt;=$F42,AE$5&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AE$5&gt;=$F42,AE$5&lt;=$F42+$G42-1),1,""))</f>
+        <f t="shared" ref="AE42:AN42" ca="1" si="20">IF(AND($C42="Goal",AE$5&gt;=$F42,AE$5&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AE$5&gt;=$F42,AE$5&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AF42" s="38" t="str">
@@ -10995,7 +10421,7 @@
         <v/>
       </c>
       <c r="AW42" s="38" t="str">
-        <f t="shared" ref="AW42:BL42" ca="1" si="21">IF(AND($C42="Goal",AW$5&gt;=$F42,AW$5&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AW$5&gt;=$F42,AW$5&lt;=$F42+$G42-1),1,""))</f>
+        <f t="shared" ref="AW42:BD42" ca="1" si="21">IF(AND($C42="Goal",AW$5&gt;=$F42,AW$5&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AW$5&gt;=$F42,AW$5&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AX42" s="38" t="str">
@@ -11059,8 +10485,8 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:64" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="66"/>
+    <row r="43" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
       <c r="B43" s="41" t="s">
         <v>87</v>
       </c>
@@ -11079,7 +10505,7 @@
       <c r="G43" s="33">
         <v>7</v>
       </c>
-      <c r="H43" s="68"/>
+      <c r="H43" s="58"/>
       <c r="I43" s="38" t="str">
         <f t="shared" ca="1" si="11"/>
         <v/>
@@ -11305,7 +10731,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="41"/>
       <c r="C44" s="34"/>
@@ -11355,7 +10781,7 @@
         <v/>
       </c>
       <c r="S44" s="38" t="str">
-        <f t="shared" ref="S44:AH44" ca="1" si="23">IF(AND($C44="Goal",S$5&gt;=$F44,S$5&lt;=$F44+$G44-1),2,IF(AND($C44="Milestone",S$5&gt;=$F44,S$5&lt;=$F44+$G44-1),1,""))</f>
+        <f t="shared" ref="S44:X44" ca="1" si="23">IF(AND($C44="Goal",S$5&gt;=$F44,S$5&lt;=$F44+$G44-1),2,IF(AND($C44="Milestone",S$5&gt;=$F44,S$5&lt;=$F44+$G44-1),1,""))</f>
         <v/>
       </c>
       <c r="T44" s="38" t="str">
@@ -11539,7 +10965,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="42" t="s">
         <v>85</v>
@@ -11775,7 +11201,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="41" t="s">
         <v>58</v>
@@ -12021,7 +11447,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="41" t="s">
         <v>59</v>
@@ -12259,9 +11685,9 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
-      <c r="B48" s="65" t="s">
+      <c r="B48" s="55" t="s">
         <v>60</v>
       </c>
       <c r="C48" s="34" t="s">
@@ -12505,9 +11931,9 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
-      <c r="B49" s="65" t="s">
+      <c r="B49" s="55" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="34" t="s">
@@ -12751,7 +12177,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="41" t="s">
         <v>62</v>
@@ -12997,7 +12423,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="41" t="s">
         <v>63</v>
@@ -13243,7 +12669,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="41" t="s">
         <v>67</v>
@@ -13489,7 +12915,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="41" t="s">
         <v>71</v>
@@ -13735,9 +13161,9 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
-      <c r="B54" s="65" t="s">
+      <c r="B54" s="55" t="s">
         <v>72</v>
       </c>
       <c r="C54" s="34" t="s">
@@ -13979,7 +13405,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="41" t="s">
         <v>70</v>
@@ -14225,7 +13651,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="41" t="s">
         <v>69</v>
@@ -14471,7 +13897,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>2</v>
       </c>
@@ -14483,231 +13909,231 @@
       <c r="G57" s="33"/>
       <c r="H57" s="26"/>
       <c r="I57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",I$5&gt;=$F57,I$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",I$5&gt;=$F57,I$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ref="I57:R58" ca="1" si="27">IF(AND($C57="Goal",I$5&gt;=$F57,I$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",I$5&gt;=$F57,I$5&lt;=$F57+$G57-1),1,""))</f>
         <v/>
       </c>
       <c r="J57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",J$5&gt;=$F57,J$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",J$5&gt;=$F57,J$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="K57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",K$5&gt;=$F57,K$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",K$5&gt;=$F57,K$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="L57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",L$5&gt;=$F57,L$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",L$5&gt;=$F57,L$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="M57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",M$5&gt;=$F57,M$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",M$5&gt;=$F57,M$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="N57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",N$5&gt;=$F57,N$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",N$5&gt;=$F57,N$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="O57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",O$5&gt;=$F57,O$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",O$5&gt;=$F57,O$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="P57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",P$5&gt;=$F57,P$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",P$5&gt;=$F57,P$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="Q57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",Q$5&gt;=$F57,Q$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",Q$5&gt;=$F57,Q$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="R57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",R$5&gt;=$F57,R$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",R$5&gt;=$F57,R$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="S57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",S$5&gt;=$F57,S$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",S$5&gt;=$F57,S$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ref="S57:AB58" ca="1" si="28">IF(AND($C57="Goal",S$5&gt;=$F57,S$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",S$5&gt;=$F57,S$5&lt;=$F57+$G57-1),1,""))</f>
         <v/>
       </c>
       <c r="T57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",T$5&gt;=$F57,T$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",T$5&gt;=$F57,T$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="U57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",U$5&gt;=$F57,U$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",U$5&gt;=$F57,U$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="V57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",V$5&gt;=$F57,V$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",V$5&gt;=$F57,V$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="W57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",W$5&gt;=$F57,W$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",W$5&gt;=$F57,W$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="X57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",X$5&gt;=$F57,X$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",X$5&gt;=$F57,X$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="Y57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",Y$5&gt;=$F57,Y$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",Y$5&gt;=$F57,Y$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="Z57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",Z$5&gt;=$F57,Z$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",Z$5&gt;=$F57,Z$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AA57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AA$5&gt;=$F57,AA$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AA$5&gt;=$F57,AA$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AB$5&gt;=$F57,AB$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AB$5&gt;=$F57,AB$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AC57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AC$5&gt;=$F57,AC$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AC$5&gt;=$F57,AC$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ref="AC57:AL58" ca="1" si="29">IF(AND($C57="Goal",AC$5&gt;=$F57,AC$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AC$5&gt;=$F57,AC$5&lt;=$F57+$G57-1),1,""))</f>
         <v/>
       </c>
       <c r="AD57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AD$5&gt;=$F57,AD$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AD$5&gt;=$F57,AD$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AE57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AE$5&gt;=$F57,AE$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AE$5&gt;=$F57,AE$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AF57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AF$5&gt;=$F57,AF$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AF$5&gt;=$F57,AF$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AG57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AG$5&gt;=$F57,AG$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AG$5&gt;=$F57,AG$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AH57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AH$5&gt;=$F57,AH$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AH$5&gt;=$F57,AH$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AI57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AI$5&gt;=$F57,AI$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AI$5&gt;=$F57,AI$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AJ57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AJ$5&gt;=$F57,AJ$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AJ$5&gt;=$F57,AJ$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AK57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AK$5&gt;=$F57,AK$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AK$5&gt;=$F57,AK$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AL57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AL$5&gt;=$F57,AL$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AL$5&gt;=$F57,AL$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AM57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AM$5&gt;=$F57,AM$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AM$5&gt;=$F57,AM$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ref="AM57:AV58" ca="1" si="30">IF(AND($C57="Goal",AM$5&gt;=$F57,AM$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AM$5&gt;=$F57,AM$5&lt;=$F57+$G57-1),1,""))</f>
         <v/>
       </c>
       <c r="AN57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AN$5&gt;=$F57,AN$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AN$5&gt;=$F57,AN$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AO57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AO$5&gt;=$F57,AO$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AO$5&gt;=$F57,AO$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AP57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AP$5&gt;=$F57,AP$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AP$5&gt;=$F57,AP$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AQ57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AQ$5&gt;=$F57,AQ$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AQ$5&gt;=$F57,AQ$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AR57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AR$5&gt;=$F57,AR$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AR$5&gt;=$F57,AR$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AS57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AS$5&gt;=$F57,AS$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AS$5&gt;=$F57,AS$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AT57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AT$5&gt;=$F57,AT$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AT$5&gt;=$F57,AT$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AU57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AU$5&gt;=$F57,AU$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AU$5&gt;=$F57,AU$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AV57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AV$5&gt;=$F57,AV$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AV$5&gt;=$F57,AV$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AW57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AW$5&gt;=$F57,AW$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AW$5&gt;=$F57,AW$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ref="AW57:BF58" ca="1" si="31">IF(AND($C57="Goal",AW$5&gt;=$F57,AW$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AW$5&gt;=$F57,AW$5&lt;=$F57+$G57-1),1,""))</f>
         <v/>
       </c>
       <c r="AX57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AX$5&gt;=$F57,AX$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AX$5&gt;=$F57,AX$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="AY57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AY$5&gt;=$F57,AY$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AY$5&gt;=$F57,AY$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="AZ57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",AZ$5&gt;=$F57,AZ$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",AZ$5&gt;=$F57,AZ$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BA57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BA$5&gt;=$F57,BA$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BA$5&gt;=$F57,BA$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BB57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BB$5&gt;=$F57,BB$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BB$5&gt;=$F57,BB$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BC57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BC$5&gt;=$F57,BC$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BC$5&gt;=$F57,BC$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BD57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BD$5&gt;=$F57,BD$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BD$5&gt;=$F57,BD$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BE57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BE$5&gt;=$F57,BE$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BE$5&gt;=$F57,BE$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BF57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BF$5&gt;=$F57,BF$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BF$5&gt;=$F57,BF$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BG57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BG$5&gt;=$F57,BG$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BG$5&gt;=$F57,BG$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ref="BG57:BL58" ca="1" si="32">IF(AND($C57="Goal",BG$5&gt;=$F57,BG$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BG$5&gt;=$F57,BG$5&lt;=$F57+$G57-1),1,""))</f>
         <v/>
       </c>
       <c r="BH57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BH$5&gt;=$F57,BH$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BH$5&gt;=$F57,BH$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BI57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BI$5&gt;=$F57,BI$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BI$5&gt;=$F57,BI$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BJ57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BJ$5&gt;=$F57,BJ$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BJ$5&gt;=$F57,BJ$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BK57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BK$5&gt;=$F57,BK$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BK$5&gt;=$F57,BK$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BL57" s="38" t="str">
-        <f ca="1">IF(AND($C57="Goal",BL$5&gt;=$F57,BL$5&lt;=$F57+$G57-1),2,IF(AND($C57="Milestone",BL$5&gt;=$F57,BL$5&lt;=$F57+$G57-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>2</v>
       </c>
@@ -14719,231 +14145,231 @@
       <c r="G58" s="33"/>
       <c r="H58" s="26"/>
       <c r="I58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",I$5&gt;=$F58,I$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",I$5&gt;=$F58,I$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="J58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",J$5&gt;=$F58,J$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",J$5&gt;=$F58,J$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="K58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",K$5&gt;=$F58,K$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",K$5&gt;=$F58,K$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="L58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",L$5&gt;=$F58,L$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",L$5&gt;=$F58,L$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="M58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",M$5&gt;=$F58,M$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",M$5&gt;=$F58,M$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="N58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",N$5&gt;=$F58,N$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",N$5&gt;=$F58,N$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="O58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",O$5&gt;=$F58,O$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",O$5&gt;=$F58,O$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="P58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",P$5&gt;=$F58,P$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",P$5&gt;=$F58,P$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="Q58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",Q$5&gt;=$F58,Q$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",Q$5&gt;=$F58,Q$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="R58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",R$5&gt;=$F58,R$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",R$5&gt;=$F58,R$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="S58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",S$5&gt;=$F58,S$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",S$5&gt;=$F58,S$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="T58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",T$5&gt;=$F58,T$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",T$5&gt;=$F58,T$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="U58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",U$5&gt;=$F58,U$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",U$5&gt;=$F58,U$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="V58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",V$5&gt;=$F58,V$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",V$5&gt;=$F58,V$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="W58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",W$5&gt;=$F58,W$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",W$5&gt;=$F58,W$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="X58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",X$5&gt;=$F58,X$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",X$5&gt;=$F58,X$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="Y58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",Y$5&gt;=$F58,Y$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",Y$5&gt;=$F58,Y$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="Z58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",Z$5&gt;=$F58,Z$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",Z$5&gt;=$F58,Z$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AA58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AA$5&gt;=$F58,AA$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AA$5&gt;=$F58,AA$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AB$5&gt;=$F58,AB$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AB$5&gt;=$F58,AB$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AC58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AC$5&gt;=$F58,AC$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AC$5&gt;=$F58,AC$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AD58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AD$5&gt;=$F58,AD$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AD$5&gt;=$F58,AD$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AE58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AE$5&gt;=$F58,AE$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AE$5&gt;=$F58,AE$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AF58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AF$5&gt;=$F58,AF$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AF$5&gt;=$F58,AF$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AG58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AG$5&gt;=$F58,AG$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AG$5&gt;=$F58,AG$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AH58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AH$5&gt;=$F58,AH$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AH$5&gt;=$F58,AH$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AI58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AI$5&gt;=$F58,AI$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AI$5&gt;=$F58,AI$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AJ58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AJ$5&gt;=$F58,AJ$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AJ$5&gt;=$F58,AJ$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AK58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AK$5&gt;=$F58,AK$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AK$5&gt;=$F58,AK$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AL58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AL$5&gt;=$F58,AL$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AL$5&gt;=$F58,AL$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AM58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AM$5&gt;=$F58,AM$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AM$5&gt;=$F58,AM$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AN58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AN$5&gt;=$F58,AN$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AN$5&gt;=$F58,AN$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AO58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AO$5&gt;=$F58,AO$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AO$5&gt;=$F58,AO$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AP58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AP$5&gt;=$F58,AP$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AP$5&gt;=$F58,AP$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AQ58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AQ$5&gt;=$F58,AQ$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AQ$5&gt;=$F58,AQ$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AR58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AR$5&gt;=$F58,AR$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AR$5&gt;=$F58,AR$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AS58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AS$5&gt;=$F58,AS$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AS$5&gt;=$F58,AS$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AT58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AT$5&gt;=$F58,AT$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AT$5&gt;=$F58,AT$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AU58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AU$5&gt;=$F58,AU$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AU$5&gt;=$F58,AU$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AV58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AV$5&gt;=$F58,AV$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AV$5&gt;=$F58,AV$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AW58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AW$5&gt;=$F58,AW$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AW$5&gt;=$F58,AW$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="AX58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AX$5&gt;=$F58,AX$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AX$5&gt;=$F58,AX$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="AY58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AY$5&gt;=$F58,AY$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AY$5&gt;=$F58,AY$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="AZ58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",AZ$5&gt;=$F58,AZ$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",AZ$5&gt;=$F58,AZ$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BA58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BA$5&gt;=$F58,BA$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BA$5&gt;=$F58,BA$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BB58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BB$5&gt;=$F58,BB$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BB$5&gt;=$F58,BB$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BC58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BC$5&gt;=$F58,BC$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BC$5&gt;=$F58,BC$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BD58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BD$5&gt;=$F58,BD$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BD$5&gt;=$F58,BD$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BE58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BE$5&gt;=$F58,BE$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BE$5&gt;=$F58,BE$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BF58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BF$5&gt;=$F58,BF$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BF$5&gt;=$F58,BF$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BG58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BG$5&gt;=$F58,BG$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BG$5&gt;=$F58,BG$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BH58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BH$5&gt;=$F58,BH$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BH$5&gt;=$F58,BH$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BI58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BI$5&gt;=$F58,BI$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BI$5&gt;=$F58,BI$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BJ58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BJ$5&gt;=$F58,BJ$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BJ$5&gt;=$F58,BJ$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BK58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BK$5&gt;=$F58,BK$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BK$5&gt;=$F58,BK$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="BL58" s="38" t="str">
-        <f ca="1">IF(AND($C58="Goal",BL$5&gt;=$F58,BL$5&lt;=$F58+$G58-1),2,IF(AND($C58="Milestone",BL$5&gt;=$F58,BL$5&lt;=$F58+$G58-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="42" t="s">
         <v>89</v>
@@ -14955,231 +14381,231 @@
       <c r="G59" s="33"/>
       <c r="H59" s="26"/>
       <c r="I59" s="38" t="str">
-        <f t="shared" ref="I59:BL63" ca="1" si="27">IF(AND($C59="Goal",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1),2,IF(AND($C59="Milestone",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1),1,""))</f>
+        <f t="shared" ref="I59:BL63" ca="1" si="33">IF(AND($C59="Goal",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1),2,IF(AND($C59="Milestone",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1),1,""))</f>
         <v/>
       </c>
       <c r="J59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="K59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="L59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="M59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="N59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="O59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="P59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Q59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="R59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="S59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="T59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="U59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="V59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="W59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="X59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Y59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Z59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AA59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AB59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AC59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AD59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AE59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AF59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AG59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AH59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AI59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AJ59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AK59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AL59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AM59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AN59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AO59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AP59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AQ59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AR59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AS59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AT59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AU59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AV59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AW59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AX59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AY59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AZ59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BA59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BB59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BC59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BD59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BE59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BF59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BG59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BH59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BI59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BJ59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BK59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BL59" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="41" t="s">
         <v>90</v>
@@ -15191,233 +14617,233 @@
       <c r="G60" s="33"/>
       <c r="H60" s="26"/>
       <c r="I60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="J60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="K60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="L60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="M60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="N60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="O60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="P60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Q60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="R60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="S60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="T60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="U60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="V60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="W60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="X60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Y60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Z60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AA60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AB60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AC60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AD60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AE60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AF60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AG60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AH60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AI60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AJ60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AK60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AL60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AM60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AN60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AO60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AP60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AQ60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AR60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AS60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AT60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AU60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AV60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AW60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AX60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AY60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AZ60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BA60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BB60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BC60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BD60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BE60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BF60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BG60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BH60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BI60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BJ60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BK60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BL60" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
-      <c r="B61" s="65" t="s">
+      <c r="B61" s="55" t="s">
         <v>91</v>
       </c>
       <c r="C61" s="34" t="s">
@@ -15437,233 +14863,233 @@
       </c>
       <c r="H61" s="26"/>
       <c r="I61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="J61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="K61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="L61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="M61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="N61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="O61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="P61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Q61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="R61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="S61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="T61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="U61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="V61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="W61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="X61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Y61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Z61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AA61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AB61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AC61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AD61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AE61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AF61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AG61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AH61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AI61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AJ61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AK61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AL61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AM61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AN61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AO61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AP61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AQ61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AR61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AS61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AT61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AU61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AV61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AW61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AX61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AY61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AZ61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BA61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BB61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BC61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BD61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BE61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BF61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BG61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BH61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BI61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BJ61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BK61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BL61" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
-      <c r="B62" s="65" t="s">
+      <c r="B62" s="55" t="s">
         <v>92</v>
       </c>
       <c r="C62" s="34" t="s">
@@ -15683,233 +15109,233 @@
       </c>
       <c r="H62" s="26"/>
       <c r="I62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="J62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="K62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="L62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="M62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="N62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="O62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="P62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Q62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="R62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="S62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="T62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="U62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="V62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="W62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="X62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Y62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Z62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AA62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AB62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AC62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AD62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AE62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AF62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AG62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AH62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AI62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AJ62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AK62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AL62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AM62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AN62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AO62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AP62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AQ62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AR62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AS62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AT62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AU62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AV62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AW62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AX62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AY62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AZ62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BA62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BB62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BC62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BD62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BE62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BF62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BG62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BH62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BI62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BJ62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BK62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BL62" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
-      <c r="B63" s="65" t="s">
+      <c r="B63" s="55" t="s">
         <v>93</v>
       </c>
       <c r="C63" s="34" t="s">
@@ -15929,231 +15355,231 @@
       </c>
       <c r="H63" s="26"/>
       <c r="I63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="J63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="K63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="L63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="M63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="N63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="O63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="P63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Q63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="R63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="S63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="T63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="U63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="V63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="W63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="X63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Y63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Z63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AA63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AB63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AC63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AD63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AE63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AF63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AG63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AH63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AI63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AJ63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AK63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AL63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AM63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AN63" s="38" t="str">
-        <f t="shared" ref="AN63:BL68" ca="1" si="28">IF(AND($C63="Goal",AN$5&gt;=$F63,AN$5&lt;=$F63+$G63-1),2,IF(AND($C63="Milestone",AN$5&gt;=$F63,AN$5&lt;=$F63+$G63-1),1,""))</f>
+        <f t="shared" ref="AN63:BL68" ca="1" si="34">IF(AND($C63="Goal",AN$5&gt;=$F63,AN$5&lt;=$F63+$G63-1),2,IF(AND($C63="Milestone",AN$5&gt;=$F63,AN$5&lt;=$F63+$G63-1),1,""))</f>
         <v/>
       </c>
       <c r="AO63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AP63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AQ63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AR63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AS63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AT63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AU63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AV63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AW63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AX63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AY63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AZ63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BA63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BB63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BC63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BD63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BE63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BF63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BG63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BH63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BI63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BJ63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BK63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BL63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="41" t="s">
         <v>97</v>
@@ -16231,7 +15657,7 @@
       <c r="BK64" s="38"/>
       <c r="BL64" s="38"/>
     </row>
-    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="41" t="s">
         <v>94</v>
@@ -16299,9 +15725,9 @@
       <c r="BK65" s="38"/>
       <c r="BL65" s="38"/>
     </row>
-    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
-      <c r="B66" s="65" t="s">
+      <c r="B66" s="55" t="s">
         <v>95</v>
       </c>
       <c r="C66" s="34" t="s">
@@ -16377,9 +15803,9 @@
       <c r="BK66" s="38"/>
       <c r="BL66" s="38"/>
     </row>
-    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
-      <c r="B67" s="65" t="s">
+      <c r="B67" s="55" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="34" t="s">
@@ -16455,7 +15881,7 @@
       <c r="BK67" s="38"/>
       <c r="BL67" s="38"/>
     </row>
-    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>2</v>
       </c>
@@ -16467,231 +15893,231 @@
       <c r="G68" s="33"/>
       <c r="H68" s="26"/>
       <c r="I68" s="38" t="str">
-        <f t="shared" ref="I68:AN68" ca="1" si="29">IF(AND($C68="Goal",I$5&gt;=$F68,I$5&lt;=$F68+$G68-1),2,IF(AND($C68="Milestone",I$5&gt;=$F68,I$5&lt;=$F68+$G68-1),1,""))</f>
+        <f t="shared" ref="I68:AN68" ca="1" si="35">IF(AND($C68="Goal",I$5&gt;=$F68,I$5&lt;=$F68+$G68-1),2,IF(AND($C68="Milestone",I$5&gt;=$F68,I$5&lt;=$F68+$G68-1),1,""))</f>
         <v/>
       </c>
       <c r="J68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="K68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="L68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="M68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="N68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="O68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="P68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="Q68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="R68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="S68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="T68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="U68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="V68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="W68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="X68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="Y68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="Z68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AA68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AB68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AC68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AD68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AE68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AF68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AG68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AH68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AI68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AJ68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AK68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AL68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AM68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AN68" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AO68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AP68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AQ68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AR68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AS68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AT68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AU68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AV68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AW68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AX68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AY68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AZ68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BA68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BB68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BC68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BD68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BE68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BF68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BG68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BH68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BI68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BJ68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BK68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BL68" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>26</v>
       </c>
@@ -16761,12 +16187,12 @@
       <c r="BK69" s="37"/>
       <c r="BL69" s="37"/>
     </row>
-    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" s="5"/>
       <c r="G70" s="16"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="6"/>
     </row>
   </sheetData>
@@ -16796,56 +16222,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:BL29 I5:BL24 I31:BL44 I46:BL56 I68:BL69">
-    <cfRule type="expression" dxfId="29" priority="54">
+    <cfRule type="expression" dxfId="33" priority="54">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AM4">
-    <cfRule type="expression" dxfId="28" priority="60">
+    <cfRule type="expression" dxfId="32" priority="60">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BL4">
-    <cfRule type="expression" dxfId="27" priority="56">
+    <cfRule type="expression" dxfId="31" priority="56">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BL4">
-    <cfRule type="expression" dxfId="26" priority="55">
+    <cfRule type="expression" dxfId="30" priority="55">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BL24 I28:BL68">
-    <cfRule type="expression" dxfId="25" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="77" stopIfTrue="1">
       <formula>AND($C8="Thomas",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="96" stopIfTrue="1">
       <formula>AND($C8="Zach",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="114" stopIfTrue="1">
       <formula>AND($C8="Jacob",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="115" stopIfTrue="1">
       <formula>AND($C8="Gage",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="116" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69:BL69">
-    <cfRule type="expression" dxfId="20" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="124" stopIfTrue="1">
       <formula>AND(#REF!="Thomas",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="125" stopIfTrue="1">
       <formula>AND(#REF!="Zach",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="126" stopIfTrue="1">
       <formula>AND(#REF!="Jacob",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="127" stopIfTrue="1">
       <formula>AND(#REF!="Gage",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="128" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16864,7 +16290,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="15" priority="46">
+    <cfRule type="expression" dxfId="19" priority="46">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16883,7 +16309,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:BL45">
-    <cfRule type="expression" dxfId="14" priority="38">
+    <cfRule type="expression" dxfId="18" priority="38">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16902,7 +16328,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:BL57">
-    <cfRule type="expression" dxfId="13" priority="30">
+    <cfRule type="expression" dxfId="17" priority="30">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16921,7 +16347,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:BL67">
-    <cfRule type="expression" dxfId="12" priority="22">
+    <cfRule type="expression" dxfId="16" priority="22">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16940,24 +16366,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:BL27">
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:BL27">
-    <cfRule type="expression" dxfId="10" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>AND($C25="Thomas",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
       <formula>AND($C25="Zach",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
       <formula>AND($C25="Jacob",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="19" stopIfTrue="1">
       <formula>AND($C25="Gage",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="20" stopIfTrue="1">
       <formula>AND(LEN($C25)=0,I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16976,46 +16402,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:BL59">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60:BL60">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:BL61">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62:BL62">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:BL67">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17037,25 +16463,23 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>63</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
@@ -17077,6 +16501,96 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>E7:E14 E31:E44 E46:E56 E68 E16:E24 E28:E29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EEB6EEE8-0D64-6C41-B789-6DDBD164946D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{49B44225-5DF1-354F-9B88-05B440CD869C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E45</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B2DE78E7-59C5-C241-A178-99859CC3B4B1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{092A2A6C-BB2A-0846-89AF-C56F25419627}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E58:E67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{96FA7B2D-FCC7-D849-A4E4-989FF21F1471}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E25:E27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2AE5C76D-1F76-7447-8843-9BBF4D25FD8A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="123" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
@@ -17117,21 +16631,6 @@
           <xm:sqref>I28:BL29 I8:BL24 I31:BL44 I46:BL56 I68:BL68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EEB6EEE8-0D64-6C41-B789-6DDBD164946D}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E30</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="53" id="{2E156086-5AF0-9941-A528-60BAC972E9B7}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -17149,21 +16648,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I30:BL30</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{49B44225-5DF1-354F-9B88-05B440CD869C}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="45" id="{DE1BC619-57D0-1642-A494-5A8A7278FC19}">
@@ -17185,21 +16669,6 @@
           <xm:sqref>I45:BL45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B2DE78E7-59C5-C241-A178-99859CC3B4B1}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E57</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="37" id="{E9CB35D6-8717-5E42-8A08-E9F4B63F2AB8}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -17217,21 +16686,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I57:BL57</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{092A2A6C-BB2A-0846-89AF-C56F25419627}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E58:E67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="29" id="{C52C9DD6-3EE2-3547-99F0-224E7183B6AE}">
@@ -17253,21 +16707,6 @@
           <xm:sqref>I58:BL67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{96FA7B2D-FCC7-D849-A4E4-989FF21F1471}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E25:E27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="21" id="{FE1D9401-991E-4E44-AC75-5412EF78CC18}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -17285,21 +16724,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I25:BL27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2AE5C76D-1F76-7447-8843-9BBF4D25FD8A}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{B303E08E-CE40-4D4F-B034-4646BB1349E8}">
@@ -17422,19 +16846,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -17448,8 +16872,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64">
+    <row r="2" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54">
         <v>43378</v>
       </c>
       <c r="B2" t="s">
@@ -17459,8 +16883,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="64">
+    <row r="3" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54">
         <v>43383</v>
       </c>
       <c r="B3" t="s">
@@ -17470,8 +16894,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64">
+    <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54">
         <v>43385</v>
       </c>
       <c r="B4" t="s">
@@ -17481,19 +16905,33 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="64">
+    <row r="5" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54">
         <v>43388</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="64">
+    <row r="6" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54">
         <v>43389</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="64">
+    <row r="7" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54">
         <v>43390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="54">
+        <v>43414</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -17506,25 +16944,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="84.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -17534,7 +16972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
work on updating meeting logs
</commit_message>
<xml_diff>
--- a/docs/gantt/gantt 10-16-18.xlsx
+++ b/docs/gantt/gantt 10-16-18.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748EEC30-B05B-4C67-ABC0-5B940B4B34D8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8AE5BD-7666-4A44-ABBF-990D67AFC4B6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16785" yWindow="465" windowWidth="16800" windowHeight="20535" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="Meeting Logs" sheetId="13" r:id="rId2"/>
     <sheet name="About" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
   <si>
     <t>About This Template</t>
   </si>
@@ -359,22 +359,62 @@
     <t>Unit Testing</t>
   </si>
   <si>
-    <t>Sparh</t>
+    <t>Initial research, decided to continue to with pygame and to use pymunk as a physics engine</t>
   </si>
   <si>
-    <t>Gage, Jacob, Zach</t>
+    <t>Created initial class diagrams, started planning for frontend and backend</t>
   </si>
   <si>
-    <t>Thruster abstraction, Thruster Subclasses, animations</t>
+    <t>Zach, Jacob, Gage</t>
+  </si>
+  <si>
+    <t>UML diagrams finished, planned building prototype over weekend</t>
+  </si>
+  <si>
+    <t>Leep2</t>
+  </si>
+  <si>
+    <t>Added SAS for directional control, added menu, implemented fuel, created static graphics class</t>
+  </si>
+  <si>
+    <t>Discussed prototype, planned gravity implementation, general planning for next steps</t>
+  </si>
+  <si>
+    <t>Discussed gravity further, planned automated SAS, HUD, visual effects</t>
+  </si>
+  <si>
+    <t>Planned finishing documentation for code stop date, final deliverables for project 3</t>
+  </si>
+  <si>
+    <t>Discussed project 4 plan</t>
+  </si>
+  <si>
+    <t>Zach, Gage</t>
+  </si>
+  <si>
+    <t>Talked about how drawer would be implemented</t>
+  </si>
+  <si>
+    <t>Updates on drawer, use of textures and sprites and the rocket builder</t>
+  </si>
+  <si>
+    <t>Quick touch-base with each other's progress</t>
+  </si>
+  <si>
+    <t>Zach, Gage, Jacob, Thomas (Later)</t>
+  </si>
+  <si>
+    <t>Workday: Work on graphics and menu components, zooming, and trajectory calculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -773,7 +813,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -927,6 +967,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,6 +998,7 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
@@ -970,7 +1014,10 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="47">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="m/d/yy"/>
     </dxf>
@@ -1706,20 +1753,20 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="45"/>
-      <tableStyleElement type="headerRow" dxfId="44"/>
-      <tableStyleElement type="firstRowStripe" dxfId="43"/>
+      <tableStyleElement type="wholeTable" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="45"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="42"/>
-      <tableStyleElement type="headerRow" dxfId="41"/>
-      <tableStyleElement type="totalRow" dxfId="40"/>
-      <tableStyleElement type="firstColumn" dxfId="39"/>
-      <tableStyleElement type="lastColumn" dxfId="38"/>
-      <tableStyleElement type="firstRowStripe" dxfId="37"/>
-      <tableStyleElement type="secondRowStripe" dxfId="36"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="35"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="34"/>
+      <tableStyleElement type="wholeTable" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
+      <tableStyleElement type="totalRow" dxfId="41"/>
+      <tableStyleElement type="firstColumn" dxfId="40"/>
+      <tableStyleElement type="lastColumn" dxfId="39"/>
+      <tableStyleElement type="firstRowStripe" dxfId="38"/>
+      <tableStyleElement type="secondRowStripe" dxfId="37"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="36"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="35"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1882,9 +1929,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone Description" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone Description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -1899,13 +1946,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D13" totalsRowShown="0">
+  <autoFilter ref="A1:D13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Location"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Members"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Things Discussed"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Things Discussed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2179,8 +2226,8 @@
   </sheetPr>
   <dimension ref="A1:BL71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView showGridLines="0" topLeftCell="W21" zoomScale="111" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2245,39 +2292,39 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="N2" s="69" t="s">
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="N2" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="70" t="s">
+      <c r="S2" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="61" t="s">
+      <c r="X2" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="62" t="s">
+      <c r="AC2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -2287,25 +2334,25 @@
         <v>48</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="66">
+      <c r="E3" s="65"/>
+      <c r="F3" s="67">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>43378</v>
       </c>
-      <c r="G3" s="67"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -2394,13 +2441,13 @@
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>43378</v>
@@ -3265,7 +3312,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="31">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F10" s="32">
         <v>43380</v>
@@ -3757,7 +3804,7 @@
         <v>43</v>
       </c>
       <c r="E12" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="32">
         <v>43378</v>
@@ -4003,7 +4050,7 @@
         <v>77</v>
       </c>
       <c r="E13" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="32">
         <v>43378</v>
@@ -4249,7 +4296,7 @@
         <v>35</v>
       </c>
       <c r="E14" s="31">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F14" s="32">
         <v>43378</v>
@@ -4495,7 +4542,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="31">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F15" s="32">
         <v>43392</v>
@@ -4816,7 +4863,9 @@
         <v>51</v>
       </c>
       <c r="D17" s="34"/>
-      <c r="E17" s="31"/>
+      <c r="E17" s="31">
+        <v>1</v>
+      </c>
       <c r="F17" s="32">
         <v>43394</v>
       </c>
@@ -5061,7 +5110,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="31">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F18" s="32">
         <v>43386</v>
@@ -5553,7 +5602,7 @@
         <v>35</v>
       </c>
       <c r="E20" s="31">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F20" s="32">
         <v>43389</v>
@@ -6045,7 +6094,7 @@
         <v>76</v>
       </c>
       <c r="E22" s="31">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F22" s="32">
         <v>43389</v>
@@ -6369,7 +6418,7 @@
         <v>75</v>
       </c>
       <c r="E24" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="32">
         <v>43390</v>
@@ -6615,7 +6664,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="31">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="F25" s="32">
         <v>43390</v>
@@ -6693,7 +6742,7 @@
         <v>43</v>
       </c>
       <c r="E26" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="32">
         <v>43392</v>
@@ -6771,7 +6820,7 @@
         <v>77</v>
       </c>
       <c r="E27" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="32">
         <v>43390</v>
@@ -7553,7 +7602,7 @@
         <v>44</v>
       </c>
       <c r="E31" s="31">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F31" s="32">
         <v>43395</v>
@@ -7799,7 +7848,7 @@
         <v>43</v>
       </c>
       <c r="E32" s="31">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F32" s="32">
         <v>43395</v>
@@ -8285,13 +8334,13 @@
         <v>66</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>77</v>
       </c>
       <c r="E34" s="31">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F34" s="32">
         <v>43423</v>
@@ -10005,7 +10054,7 @@
         <v>35</v>
       </c>
       <c r="E41" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="32">
         <v>43399</v>
@@ -11697,7 +11746,7 @@
         <v>35</v>
       </c>
       <c r="E48" s="31">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="F48" s="32">
         <v>43395</v>
@@ -12189,7 +12238,7 @@
         <v>43</v>
       </c>
       <c r="E50" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="32">
         <v>43405</v>
@@ -16222,56 +16271,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:BL29 I5:BL24 I31:BL44 I46:BL56 I68:BL69">
-    <cfRule type="expression" dxfId="33" priority="54">
+    <cfRule type="expression" dxfId="34" priority="54">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AM4">
-    <cfRule type="expression" dxfId="32" priority="60">
+    <cfRule type="expression" dxfId="33" priority="60">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BL4">
-    <cfRule type="expression" dxfId="31" priority="56">
+    <cfRule type="expression" dxfId="32" priority="56">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BL4">
-    <cfRule type="expression" dxfId="30" priority="55">
+    <cfRule type="expression" dxfId="31" priority="55">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BL24 I28:BL68">
-    <cfRule type="expression" dxfId="29" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="77" stopIfTrue="1">
       <formula>AND($C8="Thomas",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="96" stopIfTrue="1">
       <formula>AND($C8="Zach",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="114" stopIfTrue="1">
       <formula>AND($C8="Jacob",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="115" stopIfTrue="1">
       <formula>AND($C8="Gage",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="116" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69:BL69">
-    <cfRule type="expression" dxfId="24" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="124" stopIfTrue="1">
       <formula>AND(#REF!="Thomas",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="125" stopIfTrue="1">
       <formula>AND(#REF!="Zach",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="126" stopIfTrue="1">
       <formula>AND(#REF!="Jacob",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="127" stopIfTrue="1">
       <formula>AND(#REF!="Gage",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="128" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16290,7 +16339,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="19" priority="46">
+    <cfRule type="expression" dxfId="20" priority="46">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16309,7 +16358,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:BL45">
-    <cfRule type="expression" dxfId="18" priority="38">
+    <cfRule type="expression" dxfId="19" priority="38">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16328,7 +16377,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:BL57">
-    <cfRule type="expression" dxfId="17" priority="30">
+    <cfRule type="expression" dxfId="18" priority="30">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16347,7 +16396,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:BL67">
-    <cfRule type="expression" dxfId="16" priority="22">
+    <cfRule type="expression" dxfId="17" priority="22">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16366,24 +16415,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:BL27">
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:BL27">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>AND($C25="Thomas",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>AND($C25="Zach",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="18" stopIfTrue="1">
       <formula>AND($C25="Jacob",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
       <formula>AND($C25="Gage",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
       <formula>AND(LEN($C25)=0,I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16402,36 +16451,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:BL59">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60:BL60">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:BL61">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62:BL62">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:BL67">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
@@ -16847,10 +16896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16872,7 +16921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="54">
         <v>43378</v>
       </c>
@@ -16882,8 +16931,11 @@
       <c r="C2" t="s">
         <v>36</v>
       </c>
+      <c r="D2" s="61" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="54">
         <v>43383</v>
       </c>
@@ -16892,6 +16944,9 @@
       </c>
       <c r="C3" t="s">
         <v>36</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16904,34 +16959,131 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
+      <c r="D4" s="61" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="54">
         <v>43388</v>
       </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54">
         <v>43389</v>
       </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="54">
         <v>43390</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="54">
+        <v>43392</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54">
-        <v>43414</v>
+        <v>43397</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>100</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="54">
+        <v>43399</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="72">
+        <v>43402</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="72">
+        <v>43404</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="72">
+        <v>43407</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to meeting logs
</commit_message>
<xml_diff>
--- a/docs/gantt/gantt 10-16-18.xlsx
+++ b/docs/gantt/gantt 10-16-18.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E4897B-00C0-4560-90DF-DA1072CEBFCA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="415" activeTab="1"/>
+    <workbookView xWindow="16785" yWindow="465" windowWidth="16800" windowHeight="20535" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -22,29 +18,28 @@
     <definedName name="Scrolling_Increment">Gantt!$F$4</definedName>
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
   <si>
     <t>About This Template</t>
   </si>
@@ -399,14 +394,27 @@
   <si>
     <t>Talked about how drawer would be implemented</t>
   </si>
+  <si>
+    <t>Quick touch-base with each other's progress</t>
+  </si>
+  <si>
+    <t>Updates on drawer, use of textures and sprites and the rocket builder</t>
+  </si>
+  <si>
+    <t>Zach, Gage, Jacob, Thomas (Later)</t>
+  </si>
+  <si>
+    <t>Workday: Work on graphics and menu components, zooming, and trajectory calculation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -805,7 +813,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -990,12 +998,13 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="9"/>
+    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
@@ -1003,14 +1012,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="47">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <numFmt numFmtId="165" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1743,12 +1752,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3">
+    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="46"/>
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
     </tableStyle>
-    <tableStyle name="ToDoList" pivot="0" count="9">
+    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="43"/>
       <tableStyleElement type="headerRow" dxfId="42"/>
       <tableStyleElement type="totalRow" dxfId="41"/>
@@ -1861,15 +1870,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>63</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1879,7 +1888,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1910,8 +1919,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
-  <autoFilter ref="B7:G68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
+  <autoFilter ref="B7:G68" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1920,12 +1929,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Milestone Description" dataDxfId="4"/>
-    <tableColumn id="2" name="Category" dataDxfId="3"/>
-    <tableColumn id="3" name="Assigned To" dataDxfId="2"/>
-    <tableColumn id="4" name="Progress"/>
-    <tableColumn id="5" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="6" name="No. Days" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone Description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1937,13 +1946,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D13" totalsRowShown="0">
+  <autoFilter ref="A1:D13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="Members"/>
-    <tableColumn id="4" name="Things Discussed" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Location"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Members"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Things Discussed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2211,8 +2220,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BL71"/>
@@ -2221,20 +2230,20 @@
       <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="64" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="64" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -2273,7 +2282,7 @@
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -2317,7 +2326,7 @@
       <c r="AE2" s="63"/>
       <c r="AF2" s="63"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
@@ -2336,7 +2345,7 @@
       <c r="G3" s="68"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
@@ -2428,7 +2437,7 @@
       <c r="BK4" s="44"/>
       <c r="BL4" s="44"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>43433</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2732,7 +2741,7 @@
       <c r="BK6" s="47"/>
       <c r="BL6" s="48"/>
     </row>
-    <row r="7" spans="1:64" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -2980,7 +2989,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -3047,7 +3056,7 @@
       <c r="BK8" s="36"/>
       <c r="BL8" s="36"/>
     </row>
-    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -3291,7 +3300,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="41" t="s">
         <v>29</v>
@@ -3537,7 +3546,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="52" t="s">
         <v>37</v>
@@ -3783,7 +3792,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="41" t="s">
         <v>30</v>
@@ -4029,7 +4038,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="41" t="s">
         <v>31</v>
@@ -4275,7 +4284,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="41" t="s">
         <v>32</v>
@@ -4521,7 +4530,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="41" t="s">
         <v>33</v>
@@ -4599,7 +4608,7 @@
       <c r="BK15" s="38"/>
       <c r="BL15" s="38"/>
     </row>
-    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="52" t="s">
         <v>34</v>
@@ -4845,7 +4854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="42" t="s">
         <v>28</v>
@@ -5089,7 +5098,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="41" t="s">
         <v>38</v>
@@ -5335,7 +5344,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="41" t="s">
         <v>39</v>
@@ -5581,7 +5590,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="41" t="s">
         <v>40</v>
@@ -5827,7 +5836,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="41" t="s">
         <v>41</v>
@@ -6073,7 +6082,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="52" t="s">
         <v>83</v>
@@ -6151,7 +6160,7 @@
       <c r="BK22" s="38"/>
       <c r="BL22" s="38"/>
     </row>
-    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="41" t="s">
         <v>42</v>
@@ -6397,7 +6406,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="52" t="s">
         <v>49</v>
@@ -6643,7 +6652,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="52" t="s">
         <v>50</v>
@@ -6721,7 +6730,7 @@
       <c r="BK25" s="38"/>
       <c r="BL25" s="38"/>
     </row>
-    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="41" t="s">
         <v>73</v>
@@ -6799,7 +6808,7 @@
       <c r="BK26" s="38"/>
       <c r="BL26" s="38"/>
     </row>
-    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="41" t="s">
         <v>74</v>
@@ -6877,7 +6886,7 @@
       <c r="BK27" s="38"/>
       <c r="BL27" s="38"/>
     </row>
-    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="52"/>
       <c r="C28" s="34"/>
@@ -7111,7 +7120,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="41"/>
       <c r="C29" s="34"/>
@@ -7345,7 +7354,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="42" t="s">
         <v>64</v>
@@ -7581,7 +7590,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="41" t="s">
         <v>58</v>
@@ -7827,7 +7836,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="41" t="s">
         <v>62</v>
@@ -8073,7 +8082,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="41" t="s">
         <v>65</v>
@@ -8319,7 +8328,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="41" t="s">
         <v>66</v>
@@ -8565,7 +8574,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="41" t="s">
         <v>67</v>
@@ -8811,7 +8820,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="41" t="s">
         <v>70</v>
@@ -9057,7 +9066,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="41" t="s">
         <v>68</v>
@@ -9303,7 +9312,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="55" t="s">
         <v>69</v>
@@ -9541,7 +9550,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="55" t="s">
         <v>79</v>
@@ -9787,7 +9796,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="55" t="s">
         <v>80</v>
@@ -10033,7 +10042,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="41" t="s">
         <v>81</v>
@@ -10279,7 +10288,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
       <c r="B42" s="41" t="s">
         <v>82</v>
@@ -10525,7 +10534,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
       <c r="B43" s="41" t="s">
         <v>87</v>
@@ -10771,7 +10780,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="41"/>
       <c r="C44" s="34"/>
@@ -11005,7 +11014,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="42" t="s">
         <v>85</v>
@@ -11241,7 +11250,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="41" t="s">
         <v>58</v>
@@ -11487,7 +11496,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="41" t="s">
         <v>59</v>
@@ -11725,7 +11734,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="55" t="s">
         <v>60</v>
@@ -11971,7 +11980,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="55" t="s">
         <v>61</v>
@@ -12217,7 +12226,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="41" t="s">
         <v>62</v>
@@ -12463,7 +12472,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="41" t="s">
         <v>63</v>
@@ -12709,7 +12718,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="41" t="s">
         <v>67</v>
@@ -12955,7 +12964,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="41" t="s">
         <v>71</v>
@@ -13201,7 +13210,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="55" t="s">
         <v>72</v>
@@ -13445,7 +13454,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="41" t="s">
         <v>70</v>
@@ -13691,7 +13700,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="41" t="s">
         <v>69</v>
@@ -13937,7 +13946,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>2</v>
       </c>
@@ -14173,7 +14182,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>2</v>
       </c>
@@ -14409,7 +14418,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="42" t="s">
         <v>89</v>
@@ -14645,7 +14654,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="41" t="s">
         <v>90</v>
@@ -14881,7 +14890,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="55" t="s">
         <v>91</v>
@@ -15127,7 +15136,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="55" t="s">
         <v>92</v>
@@ -15373,7 +15382,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="55" t="s">
         <v>93</v>
@@ -15619,7 +15628,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="41" t="s">
         <v>97</v>
@@ -15697,7 +15706,7 @@
       <c r="BK64" s="38"/>
       <c r="BL64" s="38"/>
     </row>
-    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="41" t="s">
         <v>94</v>
@@ -15765,7 +15774,7 @@
       <c r="BK65" s="38"/>
       <c r="BL65" s="38"/>
     </row>
-    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
       <c r="B66" s="55" t="s">
         <v>95</v>
@@ -15843,7 +15852,7 @@
       <c r="BK66" s="38"/>
       <c r="BL66" s="38"/>
     </row>
-    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="55" t="s">
         <v>96</v>
@@ -15921,7 +15930,7 @@
       <c r="BK67" s="38"/>
       <c r="BL67" s="38"/>
     </row>
-    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>2</v>
       </c>
@@ -16157,7 +16166,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>26</v>
       </c>
@@ -16227,12 +16236,12 @@
       <c r="BK69" s="37"/>
       <c r="BL69" s="37"/>
     </row>
-    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" s="5"/>
       <c r="G70" s="16"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="6"/>
     </row>
   </sheetData>
@@ -16472,16 +16481,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16503,25 +16512,23 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>63</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
@@ -16888,19 +16895,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -16914,7 +16921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="54">
         <v>43378</v>
       </c>
@@ -16928,7 +16935,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="54">
         <v>43383</v>
       </c>
@@ -16942,7 +16949,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54">
         <v>43385</v>
       </c>
@@ -16956,7 +16963,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="54">
         <v>43388</v>
       </c>
@@ -16970,7 +16977,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="54">
         <v>43389</v>
       </c>
@@ -16984,7 +16991,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="54">
         <v>43390</v>
       </c>
@@ -16998,7 +17005,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="54">
         <v>43392</v>
       </c>
@@ -17012,7 +17019,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54">
         <v>43397</v>
       </c>
@@ -17026,7 +17033,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54">
         <v>43399</v>
       </c>
@@ -17038,6 +17045,45 @@
       </c>
       <c r="D10" s="61" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="72">
+        <v>43402</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72">
+        <v>43404</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="72">
+        <v>43407</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -17050,25 +17096,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="84.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -17078,7 +17124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Meeting log is now up to date
</commit_message>
<xml_diff>
--- a/docs/gantt/gantt 10-16-18.xlsx
+++ b/docs/gantt/gantt 10-16-18.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E4897B-00C0-4560-90DF-DA1072CEBFCA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E13D23-7675-4966-BCE5-747962F19BD5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16785" yWindow="465" windowWidth="16800" windowHeight="20535" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="119">
   <si>
     <t>About This Template</t>
   </si>
@@ -405,6 +405,21 @@
   </si>
   <si>
     <t>Workday: Work on graphics and menu components, zooming, and trajectory calculation</t>
+  </si>
+  <si>
+    <t>Zach, Gage, Jacob</t>
+  </si>
+  <si>
+    <t>Workday: Testing textures and zoom, refactoring of rocket components, menu designing and interfaces for components</t>
+  </si>
+  <si>
+    <t>Worked out meeting logs</t>
+  </si>
+  <si>
+    <t>Updates and planning for frontend-backend work on rocket builder, talking of refactoring some components</t>
+  </si>
+  <si>
+    <t>Planned to meet this weekend to work, otherwise talked about colissions, fixing of components and using interfaces for them</t>
   </si>
 </sst>
 </file>
@@ -1946,8 +1961,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D13" totalsRowShown="0">
-  <autoFilter ref="A1:D13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D17" totalsRowShown="0">
+  <autoFilter ref="A1:D17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Location"/>
@@ -16896,10 +16911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17084,6 +17099,62 @@
       </c>
       <c r="D13" s="61" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="72">
+        <v>43411</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="72">
+        <v>43413</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="61" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="72">
+        <v>43414</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="72">
+        <v>43416</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated meeting logs to include up to 11/23/18
</commit_message>
<xml_diff>
--- a/docs/gantt/gantt 10-16-18.xlsx
+++ b/docs/gantt/gantt 10-16-18.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD7EC8-6D88-4C7A-A6FC-D0C1A4E7896E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="415"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -22,15 +18,12 @@
     <definedName name="Scrolling_Increment">Gantt!$F$4</definedName>
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="128">
   <si>
     <t>About This Template</t>
   </si>
@@ -440,14 +436,27 @@
   <si>
     <t>Zach/Thomas</t>
   </si>
+  <si>
+    <t>Eaton 2</t>
+  </si>
+  <si>
+    <t>Zach,Gage</t>
+  </si>
+  <si>
+    <t>Discused plans for Thanksgiving Break, HUDs, and drawing of trajectories</t>
+  </si>
+  <si>
+    <t>Worked through more HUD, more trajectory drawing, and reworked how we do documentation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -860,7 +869,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1024,6 +1033,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1052,18 +1067,13 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="9"/>
+    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
@@ -1071,14 +1081,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="47">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <numFmt numFmtId="165" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1811,12 +1821,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3">
+    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="46"/>
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
     </tableStyle>
-    <tableStyle name="ToDoList" pivot="0" count="9">
+    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="43"/>
       <tableStyleElement type="headerRow" dxfId="42"/>
       <tableStyleElement type="totalRow" dxfId="41"/>
@@ -1929,15 +1939,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>63</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1947,7 +1957,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1978,8 +1988,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
-  <autoFilter ref="B7:G68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
+  <autoFilter ref="B7:G68" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1988,12 +1998,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Milestone Description" dataDxfId="4"/>
-    <tableColumn id="2" name="Category" dataDxfId="3"/>
-    <tableColumn id="3" name="Assigned To" dataDxfId="2"/>
-    <tableColumn id="4" name="Progress"/>
-    <tableColumn id="5" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="6" name="No. Days" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone Description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2005,13 +2015,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D20" totalsRowShown="0">
-  <autoFilter ref="A1:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D22" totalsRowShown="0">
+  <autoFilter ref="A1:D22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="Members"/>
-    <tableColumn id="4" name="Things Discussed" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Location"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Members"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Things Discussed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2279,30 +2289,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BL71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="60" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="60" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="64" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="64" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -2341,7 +2351,7 @@
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -2351,41 +2361,41 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="N2" s="73" t="s">
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="N2" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="74" t="s">
+      <c r="S2" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="65" t="s">
+      <c r="X2" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="66" t="s">
+      <c r="AC2" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
+      <c r="AD2" s="68"/>
+      <c r="AE2" s="68"/>
+      <c r="AF2" s="68"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
@@ -2393,25 +2403,25 @@
         <v>48</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="70">
+      <c r="E3" s="70"/>
+      <c r="F3" s="72">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>43378</v>
       </c>
-      <c r="G3" s="71"/>
+      <c r="G3" s="73"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="68"/>
+      <c r="E4" s="70"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -2496,17 +2506,17 @@
       <c r="BK4" s="44"/>
       <c r="BL4" s="44"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>43378</v>
@@ -2732,7 +2742,7 @@
         <v>43433</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2800,7 +2810,7 @@
       <c r="BK6" s="47"/>
       <c r="BL6" s="48"/>
     </row>
-    <row r="7" spans="1:64" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -3048,7 +3058,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -3115,7 +3125,7 @@
       <c r="BK8" s="36"/>
       <c r="BL8" s="36"/>
     </row>
-    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -3359,7 +3369,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="41" t="s">
         <v>29</v>
@@ -3605,7 +3615,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="52" t="s">
         <v>37</v>
@@ -3851,7 +3861,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="41" t="s">
         <v>30</v>
@@ -4097,7 +4107,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="41" t="s">
         <v>31</v>
@@ -4343,7 +4353,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="41" t="s">
         <v>32</v>
@@ -4589,7 +4599,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="41" t="s">
         <v>33</v>
@@ -4667,7 +4677,7 @@
       <c r="BK15" s="38"/>
       <c r="BL15" s="38"/>
     </row>
-    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="52" t="s">
         <v>34</v>
@@ -4913,7 +4923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="42" t="s">
         <v>28</v>
@@ -5157,7 +5167,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="41" t="s">
         <v>38</v>
@@ -5403,7 +5413,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="41" t="s">
         <v>39</v>
@@ -5649,7 +5659,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="41" t="s">
         <v>40</v>
@@ -5895,7 +5905,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="41" t="s">
         <v>41</v>
@@ -6141,7 +6151,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="52" t="s">
         <v>83</v>
@@ -6219,7 +6229,7 @@
       <c r="BK22" s="38"/>
       <c r="BL22" s="38"/>
     </row>
-    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="41" t="s">
         <v>42</v>
@@ -6465,7 +6475,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="52" t="s">
         <v>49</v>
@@ -6711,7 +6721,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="52" t="s">
         <v>50</v>
@@ -6789,7 +6799,7 @@
       <c r="BK25" s="38"/>
       <c r="BL25" s="38"/>
     </row>
-    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="41" t="s">
         <v>73</v>
@@ -6867,7 +6877,7 @@
       <c r="BK26" s="38"/>
       <c r="BL26" s="38"/>
     </row>
-    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="41" t="s">
         <v>74</v>
@@ -6945,7 +6955,7 @@
       <c r="BK27" s="38"/>
       <c r="BL27" s="38"/>
     </row>
-    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="52"/>
       <c r="C28" s="34"/>
@@ -7179,7 +7189,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="41"/>
       <c r="C29" s="34"/>
@@ -7413,7 +7423,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="42" t="s">
         <v>64</v>
@@ -7649,7 +7659,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="63" t="s">
         <v>58</v>
@@ -7895,7 +7905,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="41" t="s">
         <v>62</v>
@@ -8141,7 +8151,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="41" t="s">
         <v>65</v>
@@ -8387,7 +8397,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="41" t="s">
         <v>66</v>
@@ -8633,7 +8643,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="63" t="s">
         <v>67</v>
@@ -8879,7 +8889,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="41" t="s">
         <v>70</v>
@@ -9125,7 +9135,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="63" t="s">
         <v>68</v>
@@ -9371,7 +9381,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="64" t="s">
         <v>69</v>
@@ -9609,7 +9619,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="64" t="s">
         <v>79</v>
@@ -9855,7 +9865,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="64" t="s">
         <v>80</v>
@@ -10101,7 +10111,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="41" t="s">
         <v>81</v>
@@ -10347,7 +10357,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
       <c r="B42" s="41" t="s">
         <v>82</v>
@@ -10593,7 +10603,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
       <c r="B43" s="63" t="s">
         <v>87</v>
@@ -10839,7 +10849,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="41"/>
       <c r="C44" s="34"/>
@@ -11073,7 +11083,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="42" t="s">
         <v>85</v>
@@ -11309,7 +11319,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="63" t="s">
         <v>58</v>
@@ -11555,7 +11565,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="41" t="s">
         <v>59</v>
@@ -11793,7 +11803,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="55" t="s">
         <v>60</v>
@@ -12039,7 +12049,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="64" t="s">
         <v>61</v>
@@ -12285,7 +12295,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="63" t="s">
         <v>62</v>
@@ -12531,7 +12541,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="41" t="s">
         <v>63</v>
@@ -12777,7 +12787,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="63" t="s">
         <v>67</v>
@@ -13023,9 +13033,9 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
-      <c r="B53" s="75" t="s">
+      <c r="B53" s="65" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="34" t="s">
@@ -13269,9 +13279,9 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
-      <c r="B54" s="76" t="s">
+      <c r="B54" s="66" t="s">
         <v>72</v>
       </c>
       <c r="C54" s="34" t="s">
@@ -13513,9 +13523,9 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
-      <c r="B55" s="75" t="s">
+      <c r="B55" s="65" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="34" t="s">
@@ -13759,9 +13769,9 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="65" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="34" t="s">
@@ -14005,7 +14015,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>2</v>
       </c>
@@ -14241,7 +14251,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>2</v>
       </c>
@@ -14477,7 +14487,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="42" t="s">
         <v>89</v>
@@ -14713,7 +14723,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="41" t="s">
         <v>90</v>
@@ -14949,7 +14959,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="64" t="s">
         <v>91</v>
@@ -15195,7 +15205,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="64" t="s">
         <v>92</v>
@@ -15441,7 +15451,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="55" t="s">
         <v>93</v>
@@ -15687,7 +15697,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="63" t="s">
         <v>97</v>
@@ -15765,7 +15775,7 @@
       <c r="BK64" s="38"/>
       <c r="BL64" s="38"/>
     </row>
-    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="63" t="s">
         <v>94</v>
@@ -15833,7 +15843,7 @@
       <c r="BK65" s="38"/>
       <c r="BL65" s="38"/>
     </row>
-    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
       <c r="B66" s="64" t="s">
         <v>95</v>
@@ -15911,7 +15921,7 @@
       <c r="BK66" s="38"/>
       <c r="BL66" s="38"/>
     </row>
-    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="64" t="s">
         <v>96</v>
@@ -15989,7 +15999,7 @@
       <c r="BK67" s="38"/>
       <c r="BL67" s="38"/>
     </row>
-    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>2</v>
       </c>
@@ -16225,7 +16235,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>26</v>
       </c>
@@ -16295,12 +16305,12 @@
       <c r="BK69" s="37"/>
       <c r="BL69" s="37"/>
     </row>
-    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" s="5"/>
       <c r="G70" s="16"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="6"/>
     </row>
   </sheetData>
@@ -16540,16 +16550,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16571,25 +16581,23 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>63</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
@@ -16956,19 +16964,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -16982,7 +16990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="54">
         <v>43378</v>
       </c>
@@ -16996,7 +17004,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="54">
         <v>43383</v>
       </c>
@@ -17010,7 +17018,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54">
         <v>43385</v>
       </c>
@@ -17024,7 +17032,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="54">
         <v>43388</v>
       </c>
@@ -17038,7 +17046,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54">
         <v>43389</v>
       </c>
@@ -17052,7 +17060,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="54">
         <v>43390</v>
       </c>
@@ -17066,7 +17074,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="54">
         <v>43392</v>
       </c>
@@ -17080,7 +17088,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54">
         <v>43397</v>
       </c>
@@ -17094,7 +17102,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54">
         <v>43399</v>
       </c>
@@ -17108,7 +17116,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="62">
         <v>43402</v>
       </c>
@@ -17122,7 +17130,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="62">
         <v>43404</v>
       </c>
@@ -17133,7 +17141,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>43407</v>
       </c>
@@ -17147,7 +17155,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62">
         <v>43411</v>
       </c>
@@ -17161,7 +17169,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="62">
         <v>43413</v>
       </c>
@@ -17175,7 +17183,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="62">
         <v>43414</v>
       </c>
@@ -17189,7 +17197,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="62">
         <v>43416</v>
       </c>
@@ -17203,7 +17211,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="62">
         <v>43417</v>
       </c>
@@ -17217,7 +17225,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="62">
         <v>43418</v>
       </c>
@@ -17231,7 +17239,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
         <v>43420</v>
       </c>
@@ -17243,6 +17251,34 @@
       </c>
       <c r="D20" s="61" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="77">
+        <v>43423</v>
+      </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="77">
+        <v>43427</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="61" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -17255,25 +17291,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="84.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -17283,7 +17319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>

</xml_diff>